<commit_message>
Site updated: 2024-08-20 23:50:05
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8390,28 +8390,28 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D234" t="n">
         <v>0</v>
       </c>
       <c r="E234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H234" t="n">
         <v>0</v>
       </c>
       <c r="I234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235">

</xml_diff>

<commit_message>
Site updated: 2024-08-21 23:44:24
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8424,28 +8424,28 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D235" t="n">
         <v>0</v>
       </c>
       <c r="E235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236">

</xml_diff>

<commit_message>
Site updated: 2024-08-23 07:21:33
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8458,28 +8458,28 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D236" t="n">
         <v>0</v>
       </c>
       <c r="E236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H236" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">

</xml_diff>

<commit_message>
Site updated: 2024-08-24 07:38:06
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8492,19 +8492,19 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D237" t="n">
         <v>0</v>
       </c>
       <c r="E237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G237" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H237" t="n">
         <v>0</v>
@@ -8513,7 +8513,7 @@
         <v>0</v>
       </c>
       <c r="J237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238">

</xml_diff>

<commit_message>
Site updated: 2024-08-27 23:41:47
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8526,28 +8526,28 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D238" t="n">
         <v>0</v>
       </c>
       <c r="E238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H238" t="n">
         <v>0</v>
       </c>
       <c r="I238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239">
@@ -8560,19 +8560,19 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D239" t="n">
         <v>0</v>
       </c>
       <c r="E239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G239" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H239" t="n">
         <v>0</v>
@@ -8581,7 +8581,7 @@
         <v>0</v>
       </c>
       <c r="J239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240">
@@ -8594,19 +8594,19 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D240" t="n">
         <v>0</v>
       </c>
       <c r="E240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G240" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H240" t="n">
         <v>0</v>
@@ -8634,13 +8634,13 @@
         <v>0</v>
       </c>
       <c r="E241" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F241" t="n">
         <v>0</v>
       </c>
       <c r="G241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H241" t="n">
         <v>0</v>
@@ -8649,7 +8649,7 @@
         <v>0</v>
       </c>
       <c r="J241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242">

</xml_diff>

<commit_message>
Site updated: 2024-08-28 23:57:08
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8662,28 +8662,28 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D242" t="n">
         <v>0</v>
       </c>
       <c r="E242" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I242" t="n">
         <v>0</v>
       </c>
       <c r="J242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243">

</xml_diff>

<commit_message>
Site updated: 2024-08-30 23:46:12
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8736,22 +8736,22 @@
         <v>0</v>
       </c>
       <c r="E244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H244" t="n">
         <v>0</v>
       </c>
       <c r="I244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245">

</xml_diff>

<commit_message>
Site updated: 2024-08-31 23:50:04
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8764,28 +8764,28 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D245" t="n">
         <v>0</v>
       </c>
       <c r="E245" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F245" t="n">
         <v>0</v>
       </c>
       <c r="G245" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H245" t="n">
         <v>0</v>
       </c>
       <c r="I245" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J245" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="246">

</xml_diff>

<commit_message>
Site updated: 2024-09-01 23:50:08
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8804,22 +8804,22 @@
         <v>0</v>
       </c>
       <c r="E246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H246" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247">

</xml_diff>

<commit_message>
Site updated: 2024-09-03 09:07:19
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8832,28 +8832,28 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D247" t="n">
         <v>0</v>
       </c>
       <c r="E247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="248">

</xml_diff>

<commit_message>
Site updated: 2024-09-03 23:50:12
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8866,28 +8866,28 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D248" t="n">
         <v>0</v>
       </c>
       <c r="E248" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F248" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G248" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H248" t="n">
         <v>0</v>
       </c>
       <c r="I248" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J248" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249">

</xml_diff>

<commit_message>
Site updated: 2024-09-04 23:50:26
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8900,28 +8900,28 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D249" t="n">
         <v>0</v>
       </c>
       <c r="E249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H249" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="250">

</xml_diff>

<commit_message>
Site updated: 2024-09-05 23:53:53
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8934,28 +8934,28 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D250" t="n">
         <v>0</v>
       </c>
       <c r="E250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H250" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251">

</xml_diff>

<commit_message>
Site updated: 2024-09-07 07:50:27
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9002,25 +9002,25 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D252" t="n">
         <v>0</v>
       </c>
       <c r="E252" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F252" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G252" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H252" t="n">
         <v>0</v>
       </c>
       <c r="I252" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J252" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-09-07 09:52:15
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -8968,19 +8968,19 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D251" t="n">
         <v>0</v>
       </c>
       <c r="E251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H251" t="n">
         <v>0</v>
@@ -8989,7 +8989,7 @@
         <v>0</v>
       </c>
       <c r="J251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252">
@@ -9023,7 +9023,7 @@
         <v>1</v>
       </c>
       <c r="J252" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="253">

</xml_diff>

<commit_message>
Site updated: 2024-09-08 20:56:35
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9017,7 +9017,7 @@
         <v>1</v>
       </c>
       <c r="H252" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I252" t="n">
         <v>1</v>
@@ -9036,28 +9036,28 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D253" t="n">
         <v>0</v>
       </c>
       <c r="E253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G253" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H253" t="n">
         <v>0</v>
       </c>
       <c r="I253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254">

</xml_diff>

<commit_message>
Site updated: 2024-09-09 23:50:01
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9070,28 +9070,28 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D254" t="n">
         <v>0</v>
       </c>
       <c r="E254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H254" t="n">
         <v>0</v>
       </c>
       <c r="I254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="255">

</xml_diff>

<commit_message>
Site updated: 2024-09-11 23:37:51
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9110,13 +9110,13 @@
         <v>0</v>
       </c>
       <c r="E255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F255" t="n">
         <v>0</v>
       </c>
       <c r="G255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H255" t="n">
         <v>0</v>
@@ -9125,7 +9125,7 @@
         <v>0</v>
       </c>
       <c r="J255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="256">
@@ -9138,28 +9138,28 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D256" t="n">
         <v>0</v>
       </c>
       <c r="E256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257">

</xml_diff>

<commit_message>
Site updated: 2024-09-13 23:52:04
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9172,16 +9172,16 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D257" t="n">
         <v>0</v>
       </c>
       <c r="E257" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F257" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G257" t="n">
         <v>0</v>
@@ -9193,7 +9193,7 @@
         <v>0</v>
       </c>
       <c r="J257" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258">
@@ -9212,22 +9212,22 @@
         <v>0</v>
       </c>
       <c r="E258" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F258" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G258" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H258" t="n">
         <v>0</v>
       </c>
       <c r="I258" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J258" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259">

</xml_diff>

<commit_message>
Site updated: 2024-09-14 23:51:16
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9240,28 +9240,28 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D259" t="n">
         <v>0</v>
       </c>
       <c r="E259" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F259" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G259" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H259" t="n">
         <v>0</v>
       </c>
       <c r="I259" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J259" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260">

</xml_diff>

<commit_message>
Site updated: 2024-09-23 16:04:21
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9274,28 +9274,28 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D260" t="n">
         <v>0</v>
       </c>
       <c r="E260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H260" t="n">
         <v>0</v>
       </c>
       <c r="I260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="261">

</xml_diff>

<commit_message>
Site updated: 2024-09-24 23:49:40
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9580,28 +9580,28 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D269" t="n">
         <v>0</v>
       </c>
       <c r="E269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270">

</xml_diff>

<commit_message>
Site updated: 2024-09-27 07:34:48
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9648,28 +9648,28 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D271" t="n">
         <v>0</v>
       </c>
       <c r="E271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I271" t="n">
         <v>0</v>
       </c>
       <c r="J271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="272">

</xml_diff>

<commit_message>
Site updated: 2024-09-27 23:42:24
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9682,28 +9682,28 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D272" t="n">
         <v>0</v>
       </c>
       <c r="E272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H272" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273">

</xml_diff>

<commit_message>
Site updated: 2024-10-04 23:51:12
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9923,25 +9923,25 @@
         <v>0</v>
       </c>
       <c r="D279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E279" t="n">
         <v>0</v>
       </c>
       <c r="F279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H279" t="n">
         <v>0</v>
       </c>
       <c r="I279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="280">

</xml_diff>

<commit_message>
Site updated: 2024-10-06 23:49:19
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -9991,25 +9991,25 @@
         <v>0</v>
       </c>
       <c r="D281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G281" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H281" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="282">

</xml_diff>

<commit_message>
Site updated: 2024-10-17 23:48:13
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -10362,28 +10362,28 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E292" t="n">
         <v>0</v>
       </c>
       <c r="F292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I292" t="n">
         <v>0</v>
       </c>
       <c r="J292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293">

</xml_diff>

<commit_message>
Site updated: 2024-10-25 10:55:14
</commit_message>
<xml_diff>
--- a/statistics/2024_life_data.xlsx
+++ b/statistics/2024_life_data.xlsx
@@ -10464,7 +10464,7 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D295" t="n">
         <v>0</v>
@@ -10473,19 +10473,19 @@
         <v>0</v>
       </c>
       <c r="F295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G295" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I295" t="n">
         <v>0</v>
       </c>
       <c r="J295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296">

</xml_diff>